<commit_message>
Creates visualisations, integrates them to tex file
</commit_message>
<xml_diff>
--- a/data/ESLO/all_selected_data/quand_questions.xlsx
+++ b/data/ESLO/all_selected_data/quand_questions.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinabonan/Desktop/GitHubRepos/parameters-corpus-work/data/ESLO/all_selected_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BEC316-880E-5B4E-95B3-675E865BE97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE6A7C6-47DB-2844-89F2-EB275A97BCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38900" yWindow="-10300" windowWidth="28800" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-67720" yWindow="-10300" windowWidth="43500" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="95" r:id="rId2"/>
-    <pivotCache cacheId="99" r:id="rId3"/>
+    <pivotCache cacheId="153" r:id="rId2"/>
+    <pivotCache cacheId="154" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2908" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2926" uniqueCount="735">
   <si>
     <t>recherche</t>
   </si>
@@ -2211,6 +2211,24 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>ex situ</t>
+  </si>
+  <si>
+    <t>non cleft interrogatives</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>est-ce que</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>in situ</t>
   </si>
 </sst>
 </file>
@@ -3135,6 +3153,1268 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="50"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-A7D8-704A-93AF-E33CC0F937D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-A7D8-704A-93AF-E33CC0F937D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-A7D8-704A-93AF-E33CC0F937D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-A7D8-704A-93AF-E33CC0F937D4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A7D8-704A-93AF-E33CC0F937D4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A7D8-704A-93AF-E33CC0F937D4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A7D8-704A-93AF-E33CC0F937D4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A7D8-704A-93AF-E33CC0F937D4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$Z$4:$AA$7</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SV</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>est-ce que</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>VS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>SV</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>in situ</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AB$4:$AB$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A7D8-704A-93AF-E33CC0F937D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="50"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:alpha val="90000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:innerShdw blurRad="114300">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:innerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d contourW="19050" prstMaterial="flat">
+                <a:contourClr>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:alpha val="90000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="40000"/>
+                    </a:schemeClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="inEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$Z$58:$AA$61</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>SV</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>est-ce que</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>VS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>SV</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ex situ</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>in situ</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AB$58:$AB$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9FAC-F94E-B08C-A4E9BD4EC0AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3176,6 +4456,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4221,6 +5581,1142 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="263">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+      <a:effectLst/>
+    </cs:defRPr>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+      <a:effectLst/>
+    </cs:defRPr>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:innerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d contourW="19050" prstMaterial="flat">
+        <a:contourClr>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="263">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+      <a:effectLst/>
+    </cs:defRPr>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="40000"/>
+          </a:schemeClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+      <a:effectLst/>
+    </cs:defRPr>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="90000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:innerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d contourW="19050" prstMaterial="flat">
+        <a:contourClr>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4295,6 +6791,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F75D03D-9C33-5AF7-165B-FBED7BD17A63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5D06858-5244-7DB0-F6B5-512265728AE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5639,8 +8207,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16DAF830-211C-C44C-9B96-82533ABC4D50}" name="PivotTable7" cacheId="99" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="M57:N65" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4D41D870-F643-D44B-8967-72DE40DB25F5}" name="PivotTable6" cacheId="153" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="M3:N11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="3">
@@ -5652,9 +8220,9 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="3"/>
-        <item x="1"/>
         <item x="2"/>
         <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -5719,8 +8287,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4D41D870-F643-D44B-8967-72DE40DB25F5}" name="PivotTable6" cacheId="95" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="M3:N11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{16DAF830-211C-C44C-9B96-82533ABC4D50}" name="PivotTable7" cacheId="154" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="M57:N65" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" dataField="1" showAll="0">
       <items count="3">
@@ -5732,9 +8300,9 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="3"/>
+        <item x="1"/>
         <item x="2"/>
         <item x="0"/>
-        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6083,10 +8651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N322"/>
+  <dimension ref="A1:AB322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="U84" sqref="U84"/>
+    <sheetView tabSelected="1" topLeftCell="G33" workbookViewId="0">
+      <selection activeCell="AE56" sqref="AE56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6095,7 +8663,7 @@
     <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -6127,7 +8695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6159,7 +8727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -6196,8 +8764,11 @@
       <c r="N3" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AA3" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -6234,8 +8805,17 @@
       <c r="N4" s="2">
         <v>156</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z4" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -6272,8 +8852,17 @@
       <c r="N5" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z5" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>732</v>
+      </c>
+      <c r="AB5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6310,8 +8899,17 @@
       <c r="N6" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z6" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>733</v>
+      </c>
+      <c r="AB6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -6348,8 +8946,17 @@
       <c r="N7" s="2">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z7" t="s">
+        <v>734</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -6387,7 +8994,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -6425,7 +9032,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6463,7 +9070,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -6501,7 +9108,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -6533,7 +9140,7 @@
         <v>2961608</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -6565,7 +9172,7 @@
         <v>2015374</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -6597,7 +9204,7 @@
         <v>2062700</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -6629,7 +9236,7 @@
         <v>2743063</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -7685,7 +10292,7 @@
         <v>4801975</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -7717,7 +10324,7 @@
         <v>1080826</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -7749,7 +10356,7 @@
         <v>1152775</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -7781,7 +10388,7 @@
         <v>1956556</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -7813,7 +10420,7 @@
         <v>3111587</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -7845,7 +10452,7 @@
         <v>3752215</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -7877,7 +10484,7 @@
         <v>814236</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -7909,7 +10516,7 @@
         <v>891598</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -7941,7 +10548,7 @@
         <v>1534142</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -7978,8 +10585,11 @@
       <c r="N57" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="AA57" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -8016,8 +10626,17 @@
       <c r="N58" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z58" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -8054,8 +10673,17 @@
       <c r="N59" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z59" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>732</v>
+      </c>
+      <c r="AB59">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -8092,8 +10720,17 @@
       <c r="N60" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z60" t="s">
+        <v>729</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>733</v>
+      </c>
+      <c r="AB60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -8130,8 +10767,17 @@
       <c r="N61" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Z61" t="s">
+        <v>734</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>731</v>
+      </c>
+      <c r="AB61">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -8169,7 +10815,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -8207,7 +10853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>10</v>
       </c>

</xml_diff>